<commit_message>
last commit before returning to the states
</commit_message>
<xml_diff>
--- a/app/config/tables/deliveries/forms/deliveries/deliveries.xlsx
+++ b/app/config/tables/deliveries/forms/deliveries/deliveries.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="31020" windowHeight="17920" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1680" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -320,58 +320,58 @@
     <t>entitlements</t>
   </si>
   <si>
+    <t>pre-delivery</t>
+  </si>
+  <si>
+    <t>Item Pack out of authorized range! Do not distribute this item pack. Would you like to scan a different item pack?</t>
+  </si>
+  <si>
+    <t>This item pack is within authorized range. Please deliver this item pack.</t>
+  </si>
+  <si>
+    <t>Please click the pencil icon to record delivery</t>
+  </si>
+  <si>
+    <t>Please continue to the next screen if you have clicked the pencil icon to record delivery</t>
+  </si>
+  <si>
+    <t>data('is_delivered') == 'true'</t>
+  </si>
+  <si>
+    <t>Since the entitlement was successfully delivered, we will now complete a brief delivery report.</t>
+  </si>
+  <si>
+    <t>What is the name of the delivery site?</t>
+  </si>
+  <si>
+    <t>Thank you for completing the post-delivery survey. Continue to the next screen to finalize.</t>
+  </si>
+  <si>
+    <t>Since no item pack was successfully delivery, we will not fill out a post-distribution report.</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>data('is_delivered')</t>
+  </si>
+  <si>
+    <t>!data('is_delivered')</t>
+  </si>
+  <si>
+    <t>deliveries</t>
+  </si>
+  <si>
+    <t>Deliveries</t>
+  </si>
+  <si>
     <t>_id = ?</t>
   </si>
   <si>
-    <t>[data('delivery_id')]</t>
-  </si>
-  <si>
-    <t>'_id='+opendatakit.encodeURIDataElement('delivery_id')</t>
-  </si>
-  <si>
-    <t>pre-delivery</t>
-  </si>
-  <si>
-    <t>Item Pack out of authorized range! Do not distribute this item pack. Would you like to scan a different item pack?</t>
-  </si>
-  <si>
-    <t>This item pack is within authorized range. Please deliver this item pack.</t>
-  </si>
-  <si>
-    <t>Please click the pencil icon to record delivery</t>
-  </si>
-  <si>
-    <t>Please continue to the next screen if you have clicked the pencil icon to record delivery</t>
-  </si>
-  <si>
-    <t>data('is_delivered') == 'true'</t>
-  </si>
-  <si>
-    <t>Since the entitlement was successfully delivered, we will now complete a brief delivery report.</t>
-  </si>
-  <si>
-    <t>What is the name of the delivery site?</t>
-  </si>
-  <si>
-    <t>Thank you for completing the post-delivery survey. Continue to the next screen to finalize.</t>
-  </si>
-  <si>
-    <t>Since no item pack was successfully delivery, we will not fill out a post-distribution report.</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>data('is_delivered')</t>
-  </si>
-  <si>
-    <t>!data('is_delivered')</t>
-  </si>
-  <si>
-    <t>deliveries</t>
-  </si>
-  <si>
-    <t>Deliveries</t>
+    <t>[data('entitlement_id')]</t>
+  </si>
+  <si>
+    <t>'entitlement_id='+opendatakit.encodeURIDataElement('entitlement_id')</t>
   </si>
 </sst>
 </file>
@@ -571,8 +571,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -624,17 +634,27 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1119,7 +1139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1146,7 +1166,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C2" s="9"/>
     </row>
@@ -1164,7 +1184,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C4" s="9"/>
     </row>
@@ -1174,7 +1194,7 @@
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="23">
@@ -1253,8 +1273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1302,7 +1322,7 @@
         <v>57</v>
       </c>
       <c r="K1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="23">
@@ -1313,7 +1333,7 @@
       </c>
       <c r="D2" s="13"/>
       <c r="E2" s="14" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>30</v>
@@ -1502,7 +1522,7 @@
         <v>35</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G8" s="24"/>
       <c r="H8" s="25"/>
@@ -1633,7 +1653,7 @@
       <c r="D13" s="21"/>
       <c r="E13" s="22"/>
       <c r="F13" s="23" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G13" s="24"/>
       <c r="H13" s="25"/>
@@ -1662,7 +1682,7 @@
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G14" s="24"/>
       <c r="H14" s="25"/>
@@ -1739,7 +1759,7 @@
       <c r="D17" s="21"/>
       <c r="E17" s="22"/>
       <c r="F17" s="23" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G17" s="24"/>
       <c r="H17" s="25"/>
@@ -1839,7 +1859,7 @@
         <v>33</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
@@ -1901,7 +1921,7 @@
         <v>44</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G23" s="24"/>
       <c r="H23" s="25"/>
@@ -1966,7 +1986,7 @@
       <c r="I25" s="16"/>
       <c r="J25" s="16"/>
       <c r="K25" s="16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="L25" s="16"/>
       <c r="M25" s="16"/>
@@ -1990,14 +2010,14 @@
         <v>85</v>
       </c>
       <c r="F26" s="23" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G26" s="24"/>
       <c r="H26" s="25"/>
       <c r="I26" s="16"/>
       <c r="J26" s="16"/>
       <c r="K26" s="16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="L26" s="16"/>
       <c r="M26" s="16"/>
@@ -2021,7 +2041,7 @@
         <v>48</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G27" s="24"/>
       <c r="H27" s="25"/>
@@ -2084,7 +2104,7 @@
       <c r="I29" s="16"/>
       <c r="J29" s="16"/>
       <c r="K29" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="L29" s="16"/>
       <c r="M29" s="16"/>
@@ -2185,7 +2205,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="23" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G33" s="24"/>
       <c r="H33" s="25"/>
@@ -2266,10 +2286,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2314,23 +2334,21 @@
         <v>89</v>
       </c>
       <c r="E2" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="F2" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="G2" t="s">
         <v>86</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="H4" s="10"/>
+        <v>107</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Stable is and better organization
</commit_message>
<xml_diff>
--- a/app/config/tables/deliveries/forms/deliveries/deliveries.xlsx
+++ b/app/config/tables/deliveries/forms/deliveries/deliveries.xlsx
@@ -373,10 +373,10 @@
     <t>data('is_delivered') == 'true'</t>
   </si>
   <si>
-    <t>data('assigned_code') == ''</t>
-  </si>
-  <si>
     <t>{{data.assigned_code}}</t>
+  </si>
+  <si>
+    <t>data('assigned_code') === null || data('assigned_code') === undefined</t>
   </si>
 </sst>
 </file>
@@ -1366,7 +1366,7 @@
   <dimension ref="A1:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1486,7 +1486,7 @@
       <c r="D4" s="20"/>
       <c r="E4" s="21"/>
       <c r="F4" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G4" s="23"/>
       <c r="H4" s="24"/>
@@ -1509,7 +1509,7 @@
         <v>31</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>

</xml_diff>

<commit_message>
stable commit. Some CSS needs improvements, but the new row level permissions are now working. Now overrides can be manual or scan
</commit_message>
<xml_diff>
--- a/app/config/tables/deliveries/forms/deliveries/deliveries.xlsx
+++ b/app/config/tables/deliveries/forms/deliveries/deliveries.xlsx
@@ -4,17 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="40" windowWidth="25040" windowHeight="15500" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="1320" yWindow="100" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
     <sheet name="settings" sheetId="2" r:id="rId2"/>
     <sheet name="choices" sheetId="3" r:id="rId3"/>
     <sheet name="survey" sheetId="4" r:id="rId4"/>
-    <sheet name="prompt_types" sheetId="6" r:id="rId5"/>
-    <sheet name="calculates" sheetId="7" r:id="rId6"/>
-    <sheet name="properties" sheetId="8" r:id="rId7"/>
-    <sheet name="initial" sheetId="9" r:id="rId8"/>
+    <sheet name="calculates" sheetId="7" r:id="rId5"/>
+    <sheet name="properties" sheetId="8" r:id="rId6"/>
+    <sheet name="initial" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="105">
   <si>
     <t>type</t>
   </si>
@@ -139,9 +138,6 @@
     <t>else</t>
   </si>
   <si>
-    <t>async_assign_single_string</t>
-  </si>
-  <si>
     <t>pre-summary</t>
   </si>
   <si>
@@ -182,9 +178,6 @@
   </si>
   <si>
     <t>model.isSessionVariable</t>
-  </si>
-  <si>
-    <t>prompt_type_name</t>
   </si>
   <si>
     <t>Please confirm or update item pack barcode.</t>
@@ -373,10 +366,10 @@
     <t>data('is_delivered') == 'true'</t>
   </si>
   <si>
-    <t>{{data.assigned_code}}</t>
-  </si>
-  <si>
     <t>data('assigned_code') === null || data('assigned_code') === undefined</t>
+  </si>
+  <si>
+    <t>sector</t>
   </si>
 </sst>
 </file>
@@ -601,8 +594,66 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -692,7 +743,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="99">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -713,6 +764,35 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -733,6 +813,35 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1062,10 +1171,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1082,7 +1191,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23">
@@ -1090,7 +1199,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="23">
@@ -1106,7 +1215,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="23">
@@ -1122,7 +1231,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="23">
@@ -1170,7 +1279,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="23">
@@ -1186,7 +1295,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="23">
@@ -1194,7 +1303,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="23">
@@ -1202,18 +1311,26 @@
         <v>2</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="23">
       <c r="A17" s="34" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C17" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="23">
+      <c r="A18" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1258,7 +1375,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C2" s="9"/>
     </row>
@@ -1276,7 +1393,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C4" s="9"/>
     </row>
@@ -1286,7 +1403,7 @@
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="23">
@@ -1294,7 +1411,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C6" s="9"/>
     </row>
@@ -1334,7 +1451,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
@@ -1345,7 +1462,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
@@ -1363,10 +1480,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U38"/>
+  <dimension ref="A1:U37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1384,16 +1501,16 @@
   <sheetData>
     <row r="1" spans="1:21" ht="23">
       <c r="A1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="C1" s="27" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E1" s="28" t="s">
         <v>1</v>
@@ -1402,19 +1519,19 @@
         <v>23</v>
       </c>
       <c r="G1" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="I1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" t="s">
-        <v>51</v>
-      </c>
       <c r="K1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="23">
@@ -1425,7 +1542,7 @@
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>28</v>
@@ -1450,17 +1567,17 @@
       <c r="A3" s="18"/>
       <c r="B3" s="19"/>
       <c r="C3" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F3" s="22"/>
       <c r="G3" s="23"/>
       <c r="H3" s="24"/>
       <c r="I3" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J3" s="15" t="b">
         <v>1</v>
@@ -1478,18 +1595,20 @@
       <c r="U3" s="15"/>
     </row>
     <row r="4" spans="1:21" ht="23">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="20" t="s">
-        <v>27</v>
-      </c>
+      <c r="A4" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="20"/>
       <c r="D4" s="20"/>
       <c r="E4" s="21"/>
-      <c r="F4" s="22" t="s">
-        <v>105</v>
-      </c>
+      <c r="F4" s="22"/>
       <c r="G4" s="23"/>
-      <c r="H4" s="24"/>
+      <c r="H4" s="24" t="s">
+        <v>30</v>
+      </c>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
@@ -1505,22 +1624,24 @@
       <c r="U4" s="15"/>
     </row>
     <row r="5" spans="1:21" ht="23">
-      <c r="A5" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" s="20"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20" t="s">
+        <v>29</v>
+      </c>
       <c r="D5" s="20"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="22"/>
+      <c r="E5" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>80</v>
+      </c>
       <c r="G5" s="23"/>
-      <c r="H5" s="24" t="s">
-        <v>30</v>
-      </c>
+      <c r="H5" s="24"/>
       <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
+      <c r="J5" s="15" t="b">
+        <v>1</v>
+      </c>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
@@ -1537,14 +1658,14 @@
       <c r="A6" s="18"/>
       <c r="B6" s="19"/>
       <c r="C6" s="20" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="21" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="G6" s="23"/>
       <c r="H6" s="24"/>
@@ -1552,7 +1673,7 @@
       <c r="J6" s="15" t="b">
         <v>1</v>
       </c>
-      <c r="K6" s="15"/>
+      <c r="K6" s="19"/>
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
       <c r="N6" s="15"/>
@@ -1568,22 +1689,20 @@
       <c r="A7" s="18"/>
       <c r="B7" s="19"/>
       <c r="C7" s="20" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>53</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F7" s="22"/>
       <c r="G7" s="23"/>
       <c r="H7" s="24"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="K7" s="19"/>
+      <c r="I7" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
       <c r="N7" s="15"/>
@@ -1596,21 +1715,17 @@
       <c r="U7" s="15"/>
     </row>
     <row r="8" spans="1:21" ht="23">
-      <c r="A8" s="18"/>
+      <c r="A8" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="B8" s="19"/>
-      <c r="C8" s="20" t="s">
-        <v>39</v>
-      </c>
+      <c r="C8" s="20"/>
       <c r="D8" s="20"/>
-      <c r="E8" s="21" t="s">
-        <v>61</v>
-      </c>
+      <c r="E8" s="21"/>
       <c r="F8" s="22"/>
       <c r="G8" s="23"/>
       <c r="H8" s="24"/>
-      <c r="I8" s="15" t="s">
-        <v>62</v>
-      </c>
+      <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
@@ -1625,14 +1740,16 @@
       <c r="U8" s="15"/>
     </row>
     <row r="9" spans="1:21" ht="23">
-      <c r="A9" s="18" t="s">
-        <v>36</v>
-      </c>
+      <c r="A9" s="18"/>
       <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
+      <c r="C9" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="D9" s="20"/>
       <c r="E9" s="21"/>
-      <c r="F9" s="22"/>
+      <c r="F9" s="22" t="s">
+        <v>77</v>
+      </c>
       <c r="G9" s="23"/>
       <c r="H9" s="24"/>
       <c r="I9" s="15"/>
@@ -1653,17 +1770,21 @@
       <c r="A10" s="18"/>
       <c r="B10" s="19"/>
       <c r="C10" s="20" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D10" s="20"/>
-      <c r="E10" s="21"/>
+      <c r="E10" s="21" t="s">
+        <v>6</v>
+      </c>
       <c r="F10" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="24"/>
       <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
+      <c r="J10" s="15" t="b">
+        <v>1</v>
+      </c>
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
@@ -1680,14 +1801,14 @@
       <c r="A11" s="18"/>
       <c r="B11" s="19"/>
       <c r="C11" s="20" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="21" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="G11" s="23"/>
       <c r="H11" s="24"/>
@@ -1695,7 +1816,7 @@
       <c r="J11" s="15" t="b">
         <v>1</v>
       </c>
-      <c r="K11" s="15"/>
+      <c r="K11" s="19"/>
       <c r="L11" s="15"/>
       <c r="M11" s="15"/>
       <c r="N11" s="15"/>
@@ -1711,22 +1832,20 @@
       <c r="A12" s="18"/>
       <c r="B12" s="19"/>
       <c r="C12" s="20" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="22" t="s">
-        <v>53</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F12" s="22"/>
       <c r="G12" s="23"/>
       <c r="H12" s="24"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="K12" s="19"/>
+      <c r="I12" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
       <c r="L12" s="15"/>
       <c r="M12" s="15"/>
       <c r="N12" s="15"/>
@@ -1739,21 +1858,17 @@
       <c r="U12" s="15"/>
     </row>
     <row r="13" spans="1:21" ht="23">
-      <c r="A13" s="18"/>
+      <c r="A13" s="18" t="s">
+        <v>35</v>
+      </c>
       <c r="B13" s="19"/>
-      <c r="C13" s="20" t="s">
-        <v>39</v>
-      </c>
+      <c r="C13" s="20"/>
       <c r="D13" s="20"/>
-      <c r="E13" s="21" t="s">
-        <v>61</v>
-      </c>
+      <c r="E13" s="21"/>
       <c r="F13" s="22"/>
       <c r="G13" s="23"/>
       <c r="H13" s="24"/>
-      <c r="I13" s="36" t="s">
-        <v>85</v>
-      </c>
+      <c r="I13" s="15"/>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
@@ -1769,16 +1884,18 @@
     </row>
     <row r="14" spans="1:21" ht="23">
       <c r="A14" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="19"/>
+        <v>31</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>85</v>
+      </c>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
       <c r="F14" s="22"/>
       <c r="G14" s="23"/>
       <c r="H14" s="24"/>
-      <c r="I14" s="15"/>
+      <c r="I14" s="16"/>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
       <c r="L14" s="15"/>
@@ -1793,20 +1910,26 @@
       <c r="U14" s="15"/>
     </row>
     <row r="15" spans="1:21" ht="23">
-      <c r="A15" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="22"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>75</v>
+      </c>
       <c r="G15" s="23"/>
       <c r="H15" s="24"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="15"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="15" t="b">
+        <v>1</v>
+      </c>
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
@@ -1820,26 +1943,20 @@
       <c r="U15" s="15"/>
     </row>
     <row r="16" spans="1:21" ht="23">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="22" t="s">
-        <v>77</v>
-      </c>
+      <c r="A16" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
       <c r="G16" s="23"/>
       <c r="H16" s="24"/>
       <c r="I16" s="23"/>
-      <c r="J16" s="15" t="b">
-        <v>1</v>
-      </c>
+      <c r="J16" s="15"/>
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
@@ -1854,11 +1971,9 @@
     </row>
     <row r="17" spans="1:21" ht="23">
       <c r="A17" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>103</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B17" s="19"/>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
       <c r="E17" s="21"/>
@@ -1881,7 +1996,7 @@
     </row>
     <row r="18" spans="1:21" ht="23">
       <c r="A18" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="20"/>
@@ -1906,7 +2021,7 @@
     </row>
     <row r="19" spans="1:21" ht="23">
       <c r="A19" s="18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B19" s="19"/>
       <c r="C19" s="20"/>
@@ -1930,14 +2045,16 @@
       <c r="U19" s="15"/>
     </row>
     <row r="20" spans="1:21" ht="23">
-      <c r="A20" s="18" t="s">
-        <v>36</v>
-      </c>
+      <c r="A20" s="18"/>
       <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
+      <c r="C20" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="D20" s="20"/>
       <c r="E20" s="21"/>
-      <c r="F20" s="22"/>
+      <c r="F20" s="22" t="s">
+        <v>76</v>
+      </c>
       <c r="G20" s="23"/>
       <c r="H20" s="24"/>
       <c r="I20" s="23"/>
@@ -1958,12 +2075,16 @@
       <c r="A21" s="18"/>
       <c r="B21" s="19"/>
       <c r="C21" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="21"/>
+        <v>32</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>65</v>
+      </c>
       <c r="F21" s="22" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="G21" s="23"/>
       <c r="H21" s="24"/>
@@ -1982,23 +2103,17 @@
       <c r="U21" s="15"/>
     </row>
     <row r="22" spans="1:21" ht="23">
-      <c r="A22" s="18"/>
+      <c r="A22" s="18" t="s">
+        <v>35</v>
+      </c>
       <c r="B22" s="19"/>
-      <c r="C22" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="22" t="s">
-        <v>100</v>
-      </c>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="22"/>
       <c r="G22" s="23"/>
       <c r="H22" s="24"/>
-      <c r="I22" s="23"/>
+      <c r="I22" s="16"/>
       <c r="J22" s="15"/>
       <c r="K22" s="15"/>
       <c r="L22" s="15"/>
@@ -2014,16 +2129,18 @@
     </row>
     <row r="23" spans="1:21" ht="23">
       <c r="A23" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="19"/>
+        <v>31</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>102</v>
+      </c>
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
       <c r="E23" s="21"/>
       <c r="F23" s="22"/>
       <c r="G23" s="23"/>
       <c r="H23" s="24"/>
-      <c r="I23" s="16"/>
+      <c r="I23" s="15"/>
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
@@ -2038,19 +2155,21 @@
       <c r="U23" s="15"/>
     </row>
     <row r="24" spans="1:21" ht="23">
-      <c r="A24" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="C24" s="20"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="20" t="s">
+        <v>38</v>
+      </c>
       <c r="D24" s="20"/>
-      <c r="E24" s="21"/>
+      <c r="E24" s="21" t="s">
+        <v>61</v>
+      </c>
       <c r="F24" s="22"/>
       <c r="G24" s="23"/>
       <c r="H24" s="24"/>
-      <c r="I24" s="15"/>
+      <c r="I24" s="15" t="s">
+        <v>62</v>
+      </c>
       <c r="J24" s="15"/>
       <c r="K24" s="15"/>
       <c r="L24" s="15"/>
@@ -2068,18 +2187,18 @@
       <c r="A25" s="18"/>
       <c r="B25" s="19"/>
       <c r="C25" s="20" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="F25" s="22"/>
+        <v>37</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>68</v>
+      </c>
       <c r="G25" s="23"/>
       <c r="H25" s="24"/>
-      <c r="I25" s="15" t="s">
-        <v>64</v>
-      </c>
+      <c r="I25" s="15"/>
       <c r="J25" s="15"/>
       <c r="K25" s="15"/>
       <c r="L25" s="15"/>
@@ -2097,18 +2216,18 @@
       <c r="A26" s="18"/>
       <c r="B26" s="19"/>
       <c r="C26" s="20" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" s="22" t="s">
-        <v>70</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F26" s="22"/>
       <c r="G26" s="23"/>
       <c r="H26" s="24"/>
-      <c r="I26" s="15"/>
+      <c r="I26" s="15" t="s">
+        <v>39</v>
+      </c>
       <c r="J26" s="15"/>
       <c r="K26" s="15"/>
       <c r="L26" s="15"/>
@@ -2126,18 +2245,18 @@
       <c r="A27" s="18"/>
       <c r="B27" s="19"/>
       <c r="C27" s="20" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" s="22"/>
+        <v>5</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>40</v>
+      </c>
       <c r="G27" s="23"/>
       <c r="H27" s="24"/>
-      <c r="I27" s="15" t="s">
-        <v>40</v>
-      </c>
+      <c r="I27" s="15"/>
       <c r="J27" s="15"/>
       <c r="K27" s="15"/>
       <c r="L27" s="15"/>
@@ -2159,10 +2278,10 @@
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="21" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="F28" s="22" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="G28" s="23"/>
       <c r="H28" s="24"/>
@@ -2184,14 +2303,14 @@
       <c r="A29" s="18"/>
       <c r="B29" s="19"/>
       <c r="C29" s="20" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="21" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G29" s="23"/>
       <c r="H29" s="24"/>
@@ -2210,18 +2329,14 @@
       <c r="U29" s="15"/>
     </row>
     <row r="30" spans="1:21" ht="23">
-      <c r="A30" s="18"/>
+      <c r="A30" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="B30" s="19"/>
-      <c r="C30" s="20" t="s">
-        <v>27</v>
-      </c>
+      <c r="C30" s="20"/>
       <c r="D30" s="20"/>
-      <c r="E30" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="F30" s="22" t="s">
-        <v>72</v>
-      </c>
+      <c r="E30" s="21"/>
+      <c r="F30" s="22"/>
       <c r="G30" s="23"/>
       <c r="H30" s="24"/>
       <c r="I30" s="15"/>
@@ -2239,14 +2354,20 @@
       <c r="U30" s="15"/>
     </row>
     <row r="31" spans="1:21" ht="23">
-      <c r="A31" s="18" t="s">
-        <v>36</v>
-      </c>
+      <c r="A31" s="18"/>
       <c r="B31" s="19"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="22"/>
+      <c r="C31" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="22" t="s">
+        <v>42</v>
+      </c>
       <c r="G31" s="23"/>
       <c r="H31" s="24"/>
       <c r="I31" s="15"/>
@@ -2264,20 +2385,16 @@
       <c r="U31" s="15"/>
     </row>
     <row r="32" spans="1:21" ht="23">
-      <c r="A32" s="18"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="E32" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="F32" s="22" t="s">
-        <v>43</v>
-      </c>
+      <c r="A32" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="22"/>
       <c r="G32" s="23"/>
       <c r="H32" s="24"/>
       <c r="I32" s="15"/>
@@ -2296,11 +2413,9 @@
     </row>
     <row r="33" spans="1:21" ht="23">
       <c r="A33" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="19" t="s">
-        <v>103</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B33" s="19"/>
       <c r="C33" s="20"/>
       <c r="D33" s="20"/>
       <c r="E33" s="21"/>
@@ -2323,7 +2438,7 @@
     </row>
     <row r="34" spans="1:21" ht="23">
       <c r="A34" s="18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="20"/>
@@ -2347,14 +2462,18 @@
       <c r="U34" s="15"/>
     </row>
     <row r="35" spans="1:21" ht="23">
-      <c r="A35" s="18" t="s">
-        <v>36</v>
-      </c>
+      <c r="A35" s="18"/>
       <c r="B35" s="19"/>
-      <c r="C35" s="20"/>
+      <c r="C35" s="20" t="s">
+        <v>27</v>
+      </c>
       <c r="D35" s="20"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="22"/>
+      <c r="E35" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F35" s="22" t="s">
+        <v>71</v>
+      </c>
       <c r="G35" s="23"/>
       <c r="H35" s="24"/>
       <c r="I35" s="15"/>
@@ -2372,18 +2491,14 @@
       <c r="U35" s="15"/>
     </row>
     <row r="36" spans="1:21" ht="23">
-      <c r="A36" s="18"/>
+      <c r="A36" s="18" t="s">
+        <v>35</v>
+      </c>
       <c r="B36" s="19"/>
-      <c r="C36" s="20" t="s">
-        <v>27</v>
-      </c>
+      <c r="C36" s="20"/>
       <c r="D36" s="20"/>
-      <c r="E36" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F36" s="22" t="s">
-        <v>73</v>
-      </c>
+      <c r="E36" s="25"/>
+      <c r="F36" s="26"/>
       <c r="G36" s="23"/>
       <c r="H36" s="24"/>
       <c r="I36" s="15"/>
@@ -2407,8 +2522,8 @@
       <c r="B37" s="19"/>
       <c r="C37" s="20"/>
       <c r="D37" s="20"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="26"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="22"/>
       <c r="G37" s="23"/>
       <c r="H37" s="24"/>
       <c r="I37" s="15"/>
@@ -2425,31 +2540,6 @@
       <c r="T37" s="15"/>
       <c r="U37" s="15"/>
     </row>
-    <row r="38" spans="1:21" ht="23">
-      <c r="A38" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="15"/>
-      <c r="P38" s="15"/>
-      <c r="Q38" s="15"/>
-      <c r="R38" s="15"/>
-      <c r="S38" s="15"/>
-      <c r="T38" s="15"/>
-      <c r="U38" s="15"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2462,42 +2552,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:2" ht="30">
-      <c r="A1" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="45">
-      <c r="A2" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2512,26 +2566,26 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="255">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="240">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2545,7 +2599,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2557,13 +2611,13 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>93</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>0</v>
@@ -2574,19 +2628,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>89</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>91</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2599,7 +2653,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2611,7 +2665,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="38" t="s">
         <v>0</v>
@@ -2620,12 +2674,12 @@
         <v>23</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="25">
       <c r="A2" s="38" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B2" s="38"/>
       <c r="C2" s="38"/>
@@ -2633,12 +2687,12 @@
     </row>
     <row r="3" spans="1:4" ht="145">
       <c r="A3" s="38" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
       <c r="D3" s="38" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
functional demo, wouldn't hurt to do more iterations of the full module series
</commit_message>
<xml_diff>
--- a/app/config/tables/deliveries/forms/deliveries/deliveries.xlsx
+++ b/app/config/tables/deliveries/forms/deliveries/deliveries.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/redcross/app-designer/app/config/tables/deliveries/forms/deliveries/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="100" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -17,6 +22,9 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="109">
   <si>
     <t>type</t>
   </si>
@@ -369,7 +377,19 @@
     <t>data('assigned_code') === null || data('assigned_code') === undefined</t>
   </si>
   <si>
-    <t>sector</t>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>security</t>
+  </si>
+  <si>
+    <t>unverifiedUserCanCreate</t>
+  </si>
+  <si>
+    <t>filterTypeOnCreation</t>
+  </si>
+  <si>
+    <t>HIDDEN</t>
   </si>
 </sst>
 </file>
@@ -846,6 +866,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1171,19 +1196,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.33203125" customWidth="1"/>
     <col min="2" max="2" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23">
+    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1194,7 +1219,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="23">
+    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
         <v>2</v>
       </c>
@@ -1202,7 +1227,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="23">
+    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>3</v>
       </c>
@@ -1210,7 +1235,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="23">
+    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>2</v>
       </c>
@@ -1218,7 +1243,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="23">
+    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
         <v>2</v>
       </c>
@@ -1226,7 +1251,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="23">
+    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="33" t="s">
         <v>2</v>
       </c>
@@ -1234,7 +1259,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="23">
+    <row r="7" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>2</v>
       </c>
@@ -1242,7 +1267,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="23">
+    <row r="8" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
         <v>2</v>
       </c>
@@ -1250,7 +1275,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="23">
+    <row r="9" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
         <v>2</v>
       </c>
@@ -1258,7 +1283,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="23">
+    <row r="10" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A10" s="33" t="s">
         <v>2</v>
       </c>
@@ -1266,7 +1291,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="23">
+    <row r="11" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A11" s="33" t="s">
         <v>2</v>
       </c>
@@ -1274,7 +1299,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="23">
+    <row r="12" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A12" s="33" t="s">
         <v>2</v>
       </c>
@@ -1282,7 +1307,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="23">
+    <row r="13" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A13" s="33" t="s">
         <v>2</v>
       </c>
@@ -1290,7 +1315,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="23">
+    <row r="14" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A14" s="33" t="s">
         <v>2</v>
       </c>
@@ -1298,7 +1323,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="23">
+    <row r="15" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A15" s="33" t="s">
         <v>2</v>
       </c>
@@ -1306,7 +1331,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="23">
+    <row r="16" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A16" s="33" t="s">
         <v>2</v>
       </c>
@@ -1314,7 +1339,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="23">
+    <row r="17" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A17" s="34" t="s">
         <v>84</v>
       </c>
@@ -1323,24 +1348,11 @@
       </c>
       <c r="C17" t="b">
         <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="23">
-      <c r="A18" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="35" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1352,14 +1364,14 @@
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.1640625" customWidth="1"/>
     <col min="2" max="2" width="22.83203125" customWidth="1"/>
     <col min="3" max="3" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23">
+    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -1370,7 +1382,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="23">
+    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
@@ -1379,7 +1391,7 @@
       </c>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" ht="23">
+    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>17</v>
       </c>
@@ -1388,7 +1400,7 @@
       </c>
       <c r="C3" s="9"/>
     </row>
-    <row r="4" spans="1:3" ht="23">
+    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
@@ -1397,7 +1409,7 @@
       </c>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:3" ht="23">
+    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>19</v>
       </c>
@@ -1406,7 +1418,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="23">
+    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
@@ -1417,11 +1429,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1433,9 +1440,9 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1446,7 +1453,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1457,7 +1464,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1470,11 +1477,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1482,11 +1484,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
@@ -1499,7 +1501,7 @@
     <col min="9" max="9" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="23">
+    <row r="1" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>44</v>
       </c>
@@ -1534,7 +1536,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="23">
+    <row r="2" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="12" t="s">
@@ -1563,7 +1565,7 @@
       <c r="T2" s="15"/>
       <c r="U2" s="15"/>
     </row>
-    <row r="3" spans="1:21" ht="23">
+    <row r="3" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="18"/>
       <c r="B3" s="19"/>
       <c r="C3" s="20" t="s">
@@ -1594,7 +1596,7 @@
       <c r="T3" s="15"/>
       <c r="U3" s="15"/>
     </row>
-    <row r="4" spans="1:21" ht="23">
+    <row r="4" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>31</v>
       </c>
@@ -1623,7 +1625,7 @@
       <c r="T4" s="15"/>
       <c r="U4" s="15"/>
     </row>
-    <row r="5" spans="1:21" ht="23">
+    <row r="5" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="18"/>
       <c r="B5" s="19"/>
       <c r="C5" s="20" t="s">
@@ -1654,7 +1656,7 @@
       <c r="T5" s="15"/>
       <c r="U5" s="15"/>
     </row>
-    <row r="6" spans="1:21" ht="23">
+    <row r="6" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
       <c r="B6" s="19"/>
       <c r="C6" s="20" t="s">
@@ -1685,7 +1687,7 @@
       <c r="T6" s="15"/>
       <c r="U6" s="15"/>
     </row>
-    <row r="7" spans="1:21" ht="23">
+    <row r="7" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
       <c r="B7" s="19"/>
       <c r="C7" s="20" t="s">
@@ -1714,7 +1716,7 @@
       <c r="T7" s="15"/>
       <c r="U7" s="15"/>
     </row>
-    <row r="8" spans="1:21" ht="23">
+    <row r="8" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>36</v>
       </c>
@@ -1739,7 +1741,7 @@
       <c r="T8" s="15"/>
       <c r="U8" s="15"/>
     </row>
-    <row r="9" spans="1:21" ht="23">
+    <row r="9" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A9" s="18"/>
       <c r="B9" s="19"/>
       <c r="C9" s="20" t="s">
@@ -1766,7 +1768,7 @@
       <c r="T9" s="15"/>
       <c r="U9" s="15"/>
     </row>
-    <row r="10" spans="1:21" ht="23">
+    <row r="10" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="19"/>
       <c r="C10" s="20" t="s">
@@ -1797,7 +1799,7 @@
       <c r="T10" s="15"/>
       <c r="U10" s="15"/>
     </row>
-    <row r="11" spans="1:21" ht="23">
+    <row r="11" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="19"/>
       <c r="C11" s="20" t="s">
@@ -1828,7 +1830,7 @@
       <c r="T11" s="15"/>
       <c r="U11" s="15"/>
     </row>
-    <row r="12" spans="1:21" ht="23">
+    <row r="12" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="19"/>
       <c r="C12" s="20" t="s">
@@ -1857,7 +1859,7 @@
       <c r="T12" s="15"/>
       <c r="U12" s="15"/>
     </row>
-    <row r="13" spans="1:21" ht="23">
+    <row r="13" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>35</v>
       </c>
@@ -1882,7 +1884,7 @@
       <c r="T13" s="15"/>
       <c r="U13" s="15"/>
     </row>
-    <row r="14" spans="1:21" ht="23">
+    <row r="14" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>31</v>
       </c>
@@ -1909,7 +1911,7 @@
       <c r="T14" s="15"/>
       <c r="U14" s="15"/>
     </row>
-    <row r="15" spans="1:21" ht="23">
+    <row r="15" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="19"/>
       <c r="C15" s="20" t="s">
@@ -1942,7 +1944,7 @@
       <c r="T15" s="15"/>
       <c r="U15" s="15"/>
     </row>
-    <row r="16" spans="1:21" ht="23">
+    <row r="16" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>31</v>
       </c>
@@ -1969,7 +1971,7 @@
       <c r="T16" s="15"/>
       <c r="U16" s="15"/>
     </row>
-    <row r="17" spans="1:21" ht="23">
+    <row r="17" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>34</v>
       </c>
@@ -1994,7 +1996,7 @@
       <c r="T17" s="15"/>
       <c r="U17" s="15"/>
     </row>
-    <row r="18" spans="1:21" ht="23">
+    <row r="18" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
         <v>35</v>
       </c>
@@ -2019,7 +2021,7 @@
       <c r="T18" s="15"/>
       <c r="U18" s="15"/>
     </row>
-    <row r="19" spans="1:21" ht="23">
+    <row r="19" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
         <v>36</v>
       </c>
@@ -2044,7 +2046,7 @@
       <c r="T19" s="15"/>
       <c r="U19" s="15"/>
     </row>
-    <row r="20" spans="1:21" ht="23">
+    <row r="20" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="19"/>
       <c r="C20" s="20" t="s">
@@ -2071,7 +2073,7 @@
       <c r="T20" s="15"/>
       <c r="U20" s="15"/>
     </row>
-    <row r="21" spans="1:21" ht="23">
+    <row r="21" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
       <c r="B21" s="19"/>
       <c r="C21" s="20" t="s">
@@ -2102,7 +2104,7 @@
       <c r="T21" s="15"/>
       <c r="U21" s="15"/>
     </row>
-    <row r="22" spans="1:21" ht="23">
+    <row r="22" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
         <v>35</v>
       </c>
@@ -2127,7 +2129,7 @@
       <c r="T22" s="15"/>
       <c r="U22" s="15"/>
     </row>
-    <row r="23" spans="1:21" ht="23">
+    <row r="23" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
         <v>31</v>
       </c>
@@ -2154,7 +2156,7 @@
       <c r="T23" s="15"/>
       <c r="U23" s="15"/>
     </row>
-    <row r="24" spans="1:21" ht="23">
+    <row r="24" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A24" s="18"/>
       <c r="B24" s="19"/>
       <c r="C24" s="20" t="s">
@@ -2183,7 +2185,7 @@
       <c r="T24" s="15"/>
       <c r="U24" s="15"/>
     </row>
-    <row r="25" spans="1:21" ht="23">
+    <row r="25" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A25" s="18"/>
       <c r="B25" s="19"/>
       <c r="C25" s="20" t="s">
@@ -2212,7 +2214,7 @@
       <c r="T25" s="15"/>
       <c r="U25" s="15"/>
     </row>
-    <row r="26" spans="1:21" ht="23">
+    <row r="26" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A26" s="18"/>
       <c r="B26" s="19"/>
       <c r="C26" s="20" t="s">
@@ -2241,7 +2243,7 @@
       <c r="T26" s="15"/>
       <c r="U26" s="15"/>
     </row>
-    <row r="27" spans="1:21" ht="23">
+    <row r="27" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
       <c r="B27" s="19"/>
       <c r="C27" s="20" t="s">
@@ -2270,7 +2272,7 @@
       <c r="T27" s="15"/>
       <c r="U27" s="15"/>
     </row>
-    <row r="28" spans="1:21" ht="23">
+    <row r="28" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
       <c r="B28" s="19"/>
       <c r="C28" s="20" t="s">
@@ -2299,7 +2301,7 @@
       <c r="T28" s="15"/>
       <c r="U28" s="15"/>
     </row>
-    <row r="29" spans="1:21" ht="23">
+    <row r="29" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A29" s="18"/>
       <c r="B29" s="19"/>
       <c r="C29" s="20" t="s">
@@ -2328,7 +2330,7 @@
       <c r="T29" s="15"/>
       <c r="U29" s="15"/>
     </row>
-    <row r="30" spans="1:21" ht="23">
+    <row r="30" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
         <v>36</v>
       </c>
@@ -2353,7 +2355,7 @@
       <c r="T30" s="15"/>
       <c r="U30" s="15"/>
     </row>
-    <row r="31" spans="1:21" ht="23">
+    <row r="31" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A31" s="18"/>
       <c r="B31" s="19"/>
       <c r="C31" s="20" t="s">
@@ -2384,7 +2386,7 @@
       <c r="T31" s="15"/>
       <c r="U31" s="15"/>
     </row>
-    <row r="32" spans="1:21" ht="23">
+    <row r="32" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>31</v>
       </c>
@@ -2411,7 +2413,7 @@
       <c r="T32" s="15"/>
       <c r="U32" s="15"/>
     </row>
-    <row r="33" spans="1:21" ht="23">
+    <row r="33" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
         <v>34</v>
       </c>
@@ -2436,7 +2438,7 @@
       <c r="T33" s="15"/>
       <c r="U33" s="15"/>
     </row>
-    <row r="34" spans="1:21" ht="23">
+    <row r="34" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A34" s="18" t="s">
         <v>36</v>
       </c>
@@ -2461,7 +2463,7 @@
       <c r="T34" s="15"/>
       <c r="U34" s="15"/>
     </row>
-    <row r="35" spans="1:21" ht="23">
+    <row r="35" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A35" s="18"/>
       <c r="B35" s="19"/>
       <c r="C35" s="20" t="s">
@@ -2490,7 +2492,7 @@
       <c r="T35" s="15"/>
       <c r="U35" s="15"/>
     </row>
-    <row r="36" spans="1:21" ht="23">
+    <row r="36" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
         <v>35</v>
       </c>
@@ -2515,7 +2517,7 @@
       <c r="T36" s="15"/>
       <c r="U36" s="15"/>
     </row>
-    <row r="37" spans="1:21" ht="23">
+    <row r="37" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A37" s="18" t="s">
         <v>35</v>
       </c>
@@ -2543,11 +2545,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2559,12 +2556,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="67.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -2572,7 +2569,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="255">
+    <row r="2" spans="1:2" ht="272" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -2580,7 +2577,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="240">
+    <row r="3" spans="1:2" ht="256" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -2591,25 +2588,20 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>91</v>
       </c>
@@ -2626,7 +2618,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>87</v>
       </c>
@@ -2643,13 +2635,42 @@
         <v>90</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="39" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>108</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2661,9 +2682,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>44</v>
       </c>
@@ -2677,7 +2698,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="25">
+    <row r="2" spans="1:4" ht="27" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
         <v>95</v>
       </c>
@@ -2685,7 +2706,7 @@
       <c r="C2" s="38"/>
       <c r="D2" s="38"/>
     </row>
-    <row r="3" spans="1:4" ht="145">
+    <row r="3" spans="1:4" ht="157" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
         <v>96</v>
       </c>
@@ -2697,10 +2718,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
delivery callback paths, changes before may 22 demo
</commit_message>
<xml_diff>
--- a/app/config/tables/deliveries/forms/deliveries/deliveries.xlsx
+++ b/app/config/tables/deliveries/forms/deliveries/deliveries.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="460" windowWidth="48440" windowHeight="25740" tabRatio="989" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="choices" sheetId="4" r:id="rId5"/>
     <sheet name="calculates" sheetId="6" r:id="rId6"/>
     <sheet name="properties" sheetId="7" r:id="rId7"/>
-    <sheet name="initial" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="115">
   <si>
     <t>type</t>
   </si>
@@ -364,21 +363,6 @@
   </si>
   <si>
     <t>HIDDEN</t>
-  </si>
-  <si>
-    <t>display.text</t>
-  </si>
-  <si>
-    <t>comments</t>
-  </si>
-  <si>
-    <t>do section survey</t>
-  </si>
-  <si>
-    <t>goto _finalize</t>
-  </si>
-  <si>
-    <t>skips the finalize screen where the user chooses to save as incomplete or finalized and instead saves as finalized</t>
   </si>
   <si>
     <t>begin screen</t>
@@ -437,7 +421,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -457,13 +441,6 @@
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -613,10 +590,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -651,19 +628,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -673,7 +647,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1026,7 +1000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
@@ -1081,15 +1055,15 @@
     </row>
     <row r="2" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38"/>
+        <v>109</v>
+      </c>
+      <c r="B2" s="36"/>
+      <c r="C2" s="37"/>
       <c r="D2" s="18"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="41"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="40"/>
     </row>
     <row r="3" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
@@ -1101,7 +1075,7 @@
       <c r="E3" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="31" t="s">
         <v>59</v>
       </c>
       <c r="G3" s="20"/>
@@ -1130,7 +1104,7 @@
       <c r="E4" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="33"/>
+      <c r="F4" s="32"/>
       <c r="G4" s="25"/>
       <c r="H4" s="26"/>
       <c r="I4" s="11" t="s">
@@ -1154,13 +1128,13 @@
     </row>
     <row r="5" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B5" s="23"/>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="33"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="25"/>
       <c r="H5" s="26"/>
       <c r="I5" s="11"/>
@@ -1181,13 +1155,13 @@
       <c r="A6" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="30" t="s">
         <v>64</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="33"/>
+      <c r="F6" s="32"/>
       <c r="G6" s="25"/>
       <c r="H6" s="26" t="s">
         <v>65</v>
@@ -1216,8 +1190,8 @@
       <c r="E7" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="42" t="s">
-        <v>116</v>
+      <c r="F7" s="41" t="s">
+        <v>111</v>
       </c>
       <c r="G7" s="25"/>
       <c r="H7" s="26"/>
@@ -1248,7 +1222,7 @@
       <c r="E8" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="42" t="s">
+      <c r="F8" s="41" t="s">
         <v>68</v>
       </c>
       <c r="G8" s="25"/>
@@ -1280,7 +1254,7 @@
       <c r="E9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="33"/>
+      <c r="F9" s="32"/>
       <c r="G9" s="25"/>
       <c r="H9" s="26"/>
       <c r="I9" s="11" t="s">
@@ -1309,7 +1283,7 @@
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="33"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="25"/>
       <c r="H10" s="26"/>
       <c r="I10" s="11"/>
@@ -1334,7 +1308,7 @@
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="32" t="s">
         <v>71</v>
       </c>
       <c r="G11" s="25"/>
@@ -1363,7 +1337,7 @@
       <c r="E12" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="33" t="s">
+      <c r="F12" s="32" t="s">
         <v>72</v>
       </c>
       <c r="G12" s="25"/>
@@ -1395,7 +1369,7 @@
       <c r="E13" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="33" t="s">
+      <c r="F13" s="32" t="s">
         <v>68</v>
       </c>
       <c r="G13" s="25"/>
@@ -1427,7 +1401,7 @@
       <c r="E14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="33"/>
+      <c r="F14" s="32"/>
       <c r="G14" s="25"/>
       <c r="H14" s="26"/>
       <c r="I14" s="11" t="s">
@@ -1454,7 +1428,7 @@
       <c r="C15" s="24"/>
       <c r="D15" s="24"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="33"/>
+      <c r="F15" s="32"/>
       <c r="G15" s="25"/>
       <c r="H15" s="26"/>
       <c r="I15" s="11"/>
@@ -1481,10 +1455,10 @@
       <c r="C16" s="24"/>
       <c r="D16" s="24"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="33"/>
+      <c r="F16" s="32"/>
       <c r="G16" s="25"/>
       <c r="H16" s="26"/>
-      <c r="I16" s="35"/>
+      <c r="I16" s="34"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
@@ -1510,12 +1484,12 @@
       <c r="E17" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F17" s="33" t="s">
+      <c r="F17" s="32" t="s">
         <v>78</v>
       </c>
       <c r="G17" s="25"/>
       <c r="H17" s="26"/>
-      <c r="I17" s="36"/>
+      <c r="I17" s="35"/>
       <c r="J17" s="11" t="b">
         <f>TRUE()</f>
         <v>1</v>
@@ -1542,10 +1516,10 @@
       <c r="C18" s="24"/>
       <c r="D18" s="24"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="33"/>
+      <c r="F18" s="32"/>
       <c r="G18" s="25"/>
       <c r="H18" s="26"/>
-      <c r="I18" s="36"/>
+      <c r="I18" s="35"/>
       <c r="J18" s="11"/>
       <c r="K18" s="11"/>
       <c r="L18" s="11"/>
@@ -1567,10 +1541,10 @@
       <c r="C19" s="24"/>
       <c r="D19" s="24"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="33"/>
+      <c r="F19" s="32"/>
       <c r="G19" s="25"/>
       <c r="H19" s="26"/>
-      <c r="I19" s="36"/>
+      <c r="I19" s="35"/>
       <c r="J19" s="11"/>
       <c r="K19" s="11"/>
       <c r="L19" s="11"/>
@@ -1592,10 +1566,10 @@
       <c r="C20" s="24"/>
       <c r="D20" s="24"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="33"/>
+      <c r="F20" s="32"/>
       <c r="G20" s="25"/>
       <c r="H20" s="26"/>
-      <c r="I20" s="36"/>
+      <c r="I20" s="35"/>
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
@@ -1617,10 +1591,10 @@
       <c r="C21" s="24"/>
       <c r="D21" s="24"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="33"/>
+      <c r="F21" s="32"/>
       <c r="G21" s="25"/>
       <c r="H21" s="26"/>
-      <c r="I21" s="36"/>
+      <c r="I21" s="35"/>
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
       <c r="L21" s="11"/>
@@ -1642,12 +1616,12 @@
       </c>
       <c r="D22" s="24"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="33" t="s">
+      <c r="F22" s="32" t="s">
         <v>81</v>
       </c>
       <c r="G22" s="25"/>
       <c r="H22" s="26"/>
-      <c r="I22" s="36"/>
+      <c r="I22" s="35"/>
       <c r="J22" s="11"/>
       <c r="K22" s="11"/>
       <c r="L22" s="11"/>
@@ -1673,12 +1647,12 @@
       <c r="E23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="33" t="s">
+      <c r="F23" s="32" t="s">
         <v>82</v>
       </c>
       <c r="G23" s="25"/>
       <c r="H23" s="26"/>
-      <c r="I23" s="36"/>
+      <c r="I23" s="35"/>
       <c r="J23" s="11"/>
       <c r="K23" s="11"/>
       <c r="L23" s="11"/>
@@ -1700,10 +1674,10 @@
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="33"/>
+      <c r="F24" s="32"/>
       <c r="G24" s="25"/>
       <c r="H24" s="26"/>
-      <c r="I24" s="35"/>
+      <c r="I24" s="34"/>
       <c r="J24" s="11"/>
       <c r="K24" s="11"/>
       <c r="L24" s="11"/>
@@ -1722,12 +1696,12 @@
         <v>63</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C25" s="24"/>
       <c r="D25" s="24"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="33"/>
+      <c r="F25" s="32"/>
       <c r="G25" s="25"/>
       <c r="H25" s="26"/>
       <c r="I25" s="11"/>
@@ -1754,7 +1728,7 @@
       <c r="E26" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F26" s="33"/>
+      <c r="F26" s="32"/>
       <c r="G26" s="25"/>
       <c r="H26" s="26"/>
       <c r="I26" s="11" t="s">
@@ -1783,7 +1757,7 @@
       <c r="E27" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F27" s="33" t="s">
+      <c r="F27" s="32" t="s">
         <v>85</v>
       </c>
       <c r="G27" s="25"/>
@@ -1812,7 +1786,7 @@
       <c r="E28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F28" s="33"/>
+      <c r="F28" s="32"/>
       <c r="G28" s="25"/>
       <c r="H28" s="26"/>
       <c r="I28" s="11" t="s">
@@ -1841,7 +1815,7 @@
       <c r="E29" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="33" t="s">
+      <c r="F29" s="32" t="s">
         <v>87</v>
       </c>
       <c r="G29" s="25"/>
@@ -1870,7 +1844,7 @@
       <c r="E30" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F30" s="33" t="s">
+      <c r="F30" s="32" t="s">
         <v>88</v>
       </c>
       <c r="G30" s="25"/>
@@ -1899,7 +1873,7 @@
       <c r="E31" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F31" s="33" t="s">
+      <c r="F31" s="32" t="s">
         <v>90</v>
       </c>
       <c r="G31" s="25"/>
@@ -1926,7 +1900,7 @@
       <c r="C32" s="24"/>
       <c r="D32" s="24"/>
       <c r="E32" s="4"/>
-      <c r="F32" s="33"/>
+      <c r="F32" s="32"/>
       <c r="G32" s="25"/>
       <c r="H32" s="26"/>
       <c r="I32" s="11"/>
@@ -1955,7 +1929,7 @@
       <c r="E33" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F33" s="33" t="s">
+      <c r="F33" s="32" t="s">
         <v>91</v>
       </c>
       <c r="G33" s="25"/>
@@ -1984,7 +1958,7 @@
       <c r="C34" s="24"/>
       <c r="D34" s="24"/>
       <c r="E34" s="4"/>
-      <c r="F34" s="33"/>
+      <c r="F34" s="32"/>
       <c r="G34" s="25"/>
       <c r="H34" s="26"/>
       <c r="I34" s="11"/>
@@ -2009,7 +1983,7 @@
       <c r="C35" s="24"/>
       <c r="D35" s="24"/>
       <c r="E35" s="4"/>
-      <c r="F35" s="33"/>
+      <c r="F35" s="32"/>
       <c r="G35" s="25"/>
       <c r="H35" s="26"/>
       <c r="I35" s="11"/>
@@ -2034,7 +2008,7 @@
       <c r="C36" s="24"/>
       <c r="D36" s="24"/>
       <c r="E36" s="4"/>
-      <c r="F36" s="33"/>
+      <c r="F36" s="32"/>
       <c r="G36" s="25"/>
       <c r="H36" s="26"/>
       <c r="I36" s="11"/>
@@ -2061,7 +2035,7 @@
       <c r="E37" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F37" s="33" t="s">
+      <c r="F37" s="32" t="s">
         <v>93</v>
       </c>
       <c r="G37" s="25"/>
@@ -2088,7 +2062,7 @@
       <c r="C38" s="24"/>
       <c r="D38" s="24"/>
       <c r="E38" s="27"/>
-      <c r="F38" s="34"/>
+      <c r="F38" s="33"/>
       <c r="G38" s="25"/>
       <c r="H38" s="26"/>
       <c r="I38" s="11"/>
@@ -2113,7 +2087,7 @@
       <c r="C39" s="24"/>
       <c r="D39" s="24"/>
       <c r="E39" s="4"/>
-      <c r="F39" s="33"/>
+      <c r="F39" s="32"/>
       <c r="G39" s="25"/>
       <c r="H39" s="26"/>
       <c r="I39" s="11"/>
@@ -2286,7 +2260,7 @@
       <c r="A17" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="42" t="s">
         <v>21</v>
       </c>
       <c r="C17" t="b">
@@ -2297,7 +2271,7 @@
       <c r="A18" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="42" t="s">
         <v>61</v>
       </c>
       <c r="C18" t="b">
@@ -2308,7 +2282,7 @@
       <c r="A19" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="42" t="s">
         <v>67</v>
       </c>
       <c r="C19" t="b">
@@ -2316,7 +2290,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="44" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -2511,7 +2485,7 @@
       <c r="A2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="43" t="s">
         <v>44</v>
       </c>
       <c r="C2" t="s">
@@ -2522,7 +2496,7 @@
       <c r="A3" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="43" t="s">
         <v>46</v>
       </c>
       <c r="C3" t="s">
@@ -2539,7 +2513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2562,7 +2536,7 @@
         <v>95</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="288" x14ac:dyDescent="0.2">
@@ -2570,7 +2544,7 @@
         <v>96</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2668,57 +2642,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="62.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-    </row>
-    <row r="3" spans="1:4" ht="27" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30" t="s">
-        <v>113</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fix translations for basic_delivery
</commit_message>
<xml_diff>
--- a/app/config/tables/deliveries/forms/deliveries/deliveries.xlsx
+++ b/app/config/tables/deliveries/forms/deliveries/deliveries.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="89">
   <si>
     <t>clause</t>
   </si>
@@ -295,6 +295,12 @@
   </si>
   <si>
     <t>Assigned Item Pack Barcode</t>
+  </si>
+  <si>
+    <t>supply</t>
+  </si>
+  <si>
+    <t>Supply</t>
   </si>
 </sst>
 </file>
@@ -1060,7 +1066,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:B16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1245,16 +1251,21 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="15"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="15"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="15"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add old change that adds assigned_item_pack_code to deliveries table. previous commits are missing this
</commit_message>
<xml_diff>
--- a/app/config/tables/deliveries/forms/deliveries/deliveries.xlsx
+++ b/app/config/tables/deliveries/forms/deliveries/deliveries.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3200" windowWidth="28800" windowHeight="13480" tabRatio="989" activeTab="3"/>
+    <workbookView xWindow="80" yWindow="1240" windowWidth="28800" windowHeight="13480" tabRatio="989" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
   <si>
     <t>clause</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>member_id</t>
+  </si>
+  <si>
+    <t>assigned_item_pack_code</t>
   </si>
 </sst>
 </file>
@@ -272,7 +275,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -295,11 +298,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -319,6 +333,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -723,9 +739,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -855,6 +871,14 @@
         <v>25</v>
       </c>
     </row>
+    <row r="16" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -866,7 +890,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -937,7 +961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>